<commit_message>
Bailey Load Colors Fix
</commit_message>
<xml_diff>
--- a/Excel/Bailey/01.03.2022 BETMAR — загрузка.xlsx
+++ b/Excel/Bailey/01.03.2022 BETMAR — загрузка.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73F3FD5C-A620-423D-8762-AF6F4F498B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Bailey\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D847AE-43B5-47F7-9B0A-F597FC540C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BDF2411-D40D-4D90-9040-460EF0CE7EC2}"/>
   </bookViews>
@@ -4197,9 +4202,9 @@
   </sheetPr>
   <dimension ref="A1:V401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ2" sqref="AQ2:AR401"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V395" sqref="V395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22735,7 +22740,7 @@
         <v>963</v>
       </c>
       <c r="U273" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="V273" t="s">
         <v>964</v>
@@ -22803,7 +22808,7 @@
         <v>963</v>
       </c>
       <c r="U274" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="V274" t="s">
         <v>964</v>
@@ -22871,7 +22876,7 @@
         <v>963</v>
       </c>
       <c r="U275" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="V275" t="s">
         <v>964</v>
@@ -22939,7 +22944,7 @@
         <v>963</v>
       </c>
       <c r="U276" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="V276" t="s">
         <v>964</v>
@@ -23007,7 +23012,7 @@
         <v>963</v>
       </c>
       <c r="U277" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="V277" t="s">
         <v>964</v>
@@ -26871,7 +26876,7 @@
         <v>1080</v>
       </c>
       <c r="U335" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="V335" t="s">
         <v>1081</v>
@@ -26939,7 +26944,7 @@
         <v>1080</v>
       </c>
       <c r="U336" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="V336" t="s">
         <v>1081</v>
@@ -27007,7 +27012,7 @@
         <v>1080</v>
       </c>
       <c r="U337" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="V337" t="s">
         <v>1081</v>
@@ -27075,7 +27080,7 @@
         <v>1080</v>
       </c>
       <c r="U338" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="V338" t="s">
         <v>1081</v>
@@ -27143,7 +27148,7 @@
         <v>1080</v>
       </c>
       <c r="U339" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="V339" t="s">
         <v>1081</v>
@@ -28503,7 +28508,7 @@
         <v>1121</v>
       </c>
       <c r="U359" t="s">
-        <v>489</v>
+        <v>74</v>
       </c>
       <c r="V359" t="s">
         <v>1122</v>
@@ -28571,7 +28576,7 @@
         <v>1121</v>
       </c>
       <c r="U360" t="s">
-        <v>489</v>
+        <v>74</v>
       </c>
       <c r="V360" t="s">
         <v>1122</v>
@@ -28639,7 +28644,7 @@
         <v>1121</v>
       </c>
       <c r="U361" t="s">
-        <v>489</v>
+        <v>74</v>
       </c>
       <c r="V361" t="s">
         <v>1122</v>
@@ -28707,7 +28712,7 @@
         <v>1121</v>
       </c>
       <c r="U362" t="s">
-        <v>489</v>
+        <v>74</v>
       </c>
       <c r="V362" t="s">
         <v>1122</v>
@@ -28775,7 +28780,7 @@
         <v>1121</v>
       </c>
       <c r="U363" t="s">
-        <v>489</v>
+        <v>74</v>
       </c>
       <c r="V363" t="s">
         <v>1122</v>

</xml_diff>